<commit_message>
Nothing material. Commit before reverting historical data switch calculations for simplicity.
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CD86A9-D221-4A85-8E39-601C19EF3957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A0BF8E-DE9A-48E0-A527-DD021A4195D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -94,6 +95,105 @@
   </si>
   <si>
     <t>Give PV initial fraction to Wenjia to develop input for</t>
+  </si>
+  <si>
+    <t>Initialize solar size</t>
+  </si>
+  <si>
+    <t>Figure out initial sizing of storage systems.</t>
+  </si>
+  <si>
+    <t>Check calculation of load assumptions for economics (driven by what? And how related to specification of system sizing? For both historical approach and non hisotrical data approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should I just simplify the PV building unit options to only allow rooftop area, not building counts? </t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>New?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do I need this? </t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>PV Stock unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical data? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed kW or load based? </t>
+  </si>
+  <si>
+    <t>Econ or Impacts</t>
+  </si>
+  <si>
+    <t>NewCon</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Retro</t>
+  </si>
+  <si>
+    <t>building</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Load Based</t>
+  </si>
+  <si>
+    <t>Impacts</t>
+  </si>
+  <si>
+    <t>Make by date instead of a switch</t>
+  </si>
+  <si>
+    <t>Eliminate?</t>
+  </si>
+  <si>
+    <t>Make same?</t>
+  </si>
+  <si>
+    <t>Single multiplier?</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>No?</t>
+  </si>
+  <si>
+    <t>Decisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep same input format whether exists or not? Just change equations to not calculate averages if data are missing??? </t>
+  </si>
+  <si>
+    <t>Prob needs to be different methodology, especially with spatial component?</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Historical data switch??</t>
   </si>
 </sst>
 </file>
@@ -117,15 +217,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,11 +251,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -146,6 +273,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A85D8-C8EE-4352-97B4-D2BE29236177}">
-  <dimension ref="C2:E17"/>
+  <dimension ref="C2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,13 +694,244 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0280F3-1A88-45A7-A738-4DDFF9A5F04A}">
+  <dimension ref="B3:K34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="I4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit before attempting to import all new data & dimensions for NYPA specific input
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A0BF8E-DE9A-48E0-A527-DD021A4195D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C396A07C-D665-4368-B0B9-0D2AEF1D234E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>Historical data switch??</t>
+  </si>
+  <si>
+    <t>Import Spatial ID index (not All spatial ID index)</t>
+  </si>
+  <si>
+    <t>Escalate total building consumption in global data input for NYPA</t>
   </si>
 </sst>
 </file>
@@ -594,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A85D8-C8EE-4352-97B4-D2BE29236177}">
-  <dimension ref="C2:E21"/>
+  <dimension ref="C2:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +728,16 @@
         <v>23</v>
       </c>
     </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -732,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0280F3-1A88-45A7-A738-4DDFF9A5F04A}">
   <dimension ref="B3:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Imported all new NYPA data successfully for the first time.
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C396A07C-D665-4368-B0B9-0D2AEF1D234E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C53CE72-DD68-438F-A686-A58546E1FE20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Escalate total building consumption in global data input for NYPA</t>
+  </si>
+  <si>
+    <t>Check how taxes are determined to be applied</t>
+  </si>
+  <si>
+    <t>Input historical system installations &amp; capacity</t>
+  </si>
+  <si>
+    <t>Fix DC to AC ratio and factor inputs/calculations</t>
   </si>
 </sst>
 </file>
@@ -600,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A85D8-C8EE-4352-97B4-D2BE29236177}">
-  <dimension ref="C2:E23"/>
+  <dimension ref="C2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,6 +745,26 @@
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed all calculated values for DC to AC ratios into a single input table, for simplicity. Imported placeholder data for DC to AC Ratio
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C53CE72-DD68-438F-A686-A58546E1FE20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557BA33-2342-4B7B-BFEE-F40409AE98E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Fix DC to AC ratio and factor inputs/calculations</t>
+  </si>
+  <si>
+    <t>Revisit DC to AC ratio issue (is the higher loss factor appropriate for econ analysis?)</t>
   </si>
 </sst>
 </file>
@@ -609,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A85D8-C8EE-4352-97B4-D2BE29236177}">
-  <dimension ref="C2:E27"/>
+  <dimension ref="C2:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,6 +768,11 @@
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified key electric rate maps to calculate existing electric rates by sector.
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8557BA33-2342-4B7B-BFEE-F40409AE98E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4535A2D-5B3A-4652-9F9A-C28DBFC2386A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -212,6 +213,66 @@
   </si>
   <si>
     <t>Revisit DC to AC ratio issue (is the higher loss factor appropriate for econ analysis?)</t>
+  </si>
+  <si>
+    <t>Input action</t>
+  </si>
+  <si>
+    <t>Develop representative electric rates</t>
+  </si>
+  <si>
+    <t>Electric Rates</t>
+  </si>
+  <si>
+    <t>Select start periods for each rate vintage</t>
+  </si>
+  <si>
+    <t>Relevant model node</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Why is solar new construction type not simulating (see PV Cumulative Adoption)</t>
+  </si>
+  <si>
+    <t>Run Battery Optimization</t>
+  </si>
+  <si>
+    <t>Develop initial storage inputs</t>
+  </si>
+  <si>
+    <t>Develop initial PV input capacity &amp; installation quantity</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>PV Inputs</t>
+  </si>
+  <si>
+    <t>Develop PV logit coefficients</t>
+  </si>
+  <si>
+    <t>Create outputs for energy, MW, avoided GHG</t>
+  </si>
+  <si>
+    <t>Develop GHG input assumptions</t>
+  </si>
+  <si>
+    <t>Add input to reduce market for NYPA accessible</t>
+  </si>
+  <si>
+    <t>Develop community solar strategy for output</t>
+  </si>
+  <si>
+    <t>Adjust inputs &amp; logic to account for land and/or parking lot area</t>
+  </si>
+  <si>
+    <t>Align scaling, system sizes, loads &amp; understand</t>
+  </si>
+  <si>
+    <t>Logic</t>
   </si>
 </sst>
 </file>
@@ -612,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6A85D8-C8EE-4352-97B4-D2BE29236177}">
-  <dimension ref="C2:E28"/>
+  <dimension ref="C2:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +834,11 @@
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -987,4 +1053,113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AB9A82-62F0-45FC-9CEF-1A59FDF3A54E}">
+  <dimension ref="B5:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First crack at inputting manually the historical PV interconnections (unsuccessfully so far)
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4535A2D-5B3A-4652-9F9A-C28DBFC2386A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC43E396-3F97-4D5B-8F3E-1674D9AD2B20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Logic</t>
+  </si>
+  <si>
+    <t>Check input and logic for hourly load profiles to see if they have to be average per building</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AB9A82-62F0-45FC-9CEF-1A59FDF3A54E}">
-  <dimension ref="B5:D17"/>
+  <dimension ref="B5:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,6 +1162,11 @@
         <v>77</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed all load scaling inputs to ensure loads are indexed by PV climate and consistent with PV system sizing calculations.
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC43E396-3F97-4D5B-8F3E-1674D9AD2B20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC76D22-AFB6-4998-8001-F1CD017D4A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Check input and logic for hourly load profiles to see if they have to be average per building</t>
+  </si>
+  <si>
+    <t>Change load scaling for economics to be by climate zone, for consistency with PV generation by climate zone</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AB9A82-62F0-45FC-9CEF-1A59FDF3A54E}">
-  <dimension ref="B5:D18"/>
+  <dimension ref="B5:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,6 +1170,11 @@
         <v>79</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Moved files changed from commit fdd4af5 to here to skip over the accidental large file commit.
</commit_message>
<xml_diff>
--- a/TTD.xlsx
+++ b/TTD.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC76D22-AFB6-4998-8001-F1CD017D4A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF31D77-2429-4796-A971-5A9C0136E630}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8D9A275E-18D4-4F19-9805-038BEAC18461}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
   <si>
     <t>Import/define All_pv_sectors</t>
   </si>
@@ -113,90 +112,6 @@
     <t>asdf</t>
   </si>
   <si>
-    <t>New?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do I need this? </t>
-  </si>
-  <si>
-    <t>Vintage</t>
-  </si>
-  <si>
-    <t>PV Stock unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Historical data? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixed kW or load based? </t>
-  </si>
-  <si>
-    <t>Econ or Impacts</t>
-  </si>
-  <si>
-    <t>NewCon</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Retro</t>
-  </si>
-  <si>
-    <t>building</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Load Based</t>
-  </si>
-  <si>
-    <t>Impacts</t>
-  </si>
-  <si>
-    <t>Make by date instead of a switch</t>
-  </si>
-  <si>
-    <t>Eliminate?</t>
-  </si>
-  <si>
-    <t>Make same?</t>
-  </si>
-  <si>
-    <t>Single multiplier?</t>
-  </si>
-  <si>
-    <t>Keep</t>
-  </si>
-  <si>
-    <t>No?</t>
-  </si>
-  <si>
-    <t>Decisions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keep same input format whether exists or not? Just change equations to not calculate averages if data are missing??? </t>
-  </si>
-  <si>
-    <t>Prob needs to be different methodology, especially with spatial component?</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Historical data switch??</t>
-  </si>
-  <si>
     <t>Import Spatial ID index (not All spatial ID index)</t>
   </si>
   <si>
@@ -227,9 +142,6 @@
     <t>Select start periods for each rate vintage</t>
   </si>
   <si>
-    <t>Relevant model node</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -279,6 +191,66 @@
   </si>
   <si>
     <t>Change load scaling for economics to be by climate zone, for consistency with PV generation by climate zone</t>
+  </si>
+  <si>
+    <t>Review solar PV costs. They look high for larger nonresidential installations</t>
+  </si>
+  <si>
+    <t>Review storage costs. Appropriate for larger installs?</t>
+  </si>
+  <si>
+    <t>Develop strategy for using land/parking area in our estimates</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Wenjia?</t>
+  </si>
+  <si>
+    <t>Talk to Rush about what he's looked up. Look at Joe's electric rate files (not especially helpful)</t>
+  </si>
+  <si>
+    <t>Cory</t>
+  </si>
+  <si>
+    <t>Global Inputs</t>
+  </si>
+  <si>
+    <t>Wenjia</t>
+  </si>
+  <si>
+    <t>Storage Inputs</t>
+  </si>
+  <si>
+    <t>Research and develop rough estimate for battery capacity (MW) relative to Peak customer load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcion of PV system sizing, rather?? </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Revise logit cost ratio logic (only system vs. grid)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Cory/Wenjia</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Included in roof area or no?</t>
+  </si>
+  <si>
+    <t>Check whether to just use decision variables, or whether to input appropriate coefficients into stored nodes</t>
+  </si>
+  <si>
+    <t>Look at all "saved" storage decision variables and which decision variables are included in the optimization and ensure they are consistent</t>
   </si>
 </sst>
 </file>
@@ -302,33 +274,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -336,20 +290,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -358,13 +303,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,7 +620,7 @@
   <dimension ref="C2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,46 +653,73 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
@@ -763,21 +728,33 @@
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
@@ -809,17 +786,17 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
@@ -829,22 +806,22 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -854,328 +831,304 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0280F3-1A88-45A7-A738-4DDFF9A5F04A}">
-  <dimension ref="B3:K34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="J3" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AB9A82-62F0-45FC-9CEF-1A59FDF3A54E}">
-  <dimension ref="B5:D19"/>
+  <dimension ref="B5:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="61.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="3" max="3" width="97.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="87.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="C27" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>80</v>
+      <c r="D27" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>